<commit_message>
update currency payhelp and transportation
</commit_message>
<xml_diff>
--- a/NhapHangV2.API/Template/MainOrderReportTemplate.xlsx
+++ b/NhapHangV2.API/Template/MainOrderReportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mona\nhaphangv2.monamedia.net\NhapHangV2.API\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MonaMedia\nhaphang.monamedia.net\NhapHangV2.API\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9D9F8F-8D0B-4538-8ED4-0EB85FD0A97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1447F485-C613-4211-9C42-F6626B6820D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{56308B7F-08DD-4126-B811-B99ED4BE5686}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{56308B7F-08DD-4126-B811-B99ED4BE5686}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>MÃ ĐƠN HÀNG</t>
   </si>
@@ -43,9 +43,6 @@
     <t>USERNAME</t>
   </si>
   <si>
-    <t>TÊN SHOP</t>
-  </si>
-  <si>
     <t>NV KINH DOANH</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>[[%Field:Id%]]</t>
   </si>
   <si>
-    <t>[[%Field:ShopName%]]</t>
-  </si>
-  <si>
     <t>[[%Field:SalerUserName%]]</t>
   </si>
   <si>
@@ -119,6 +113,24 @@
   </si>
   <si>
     <t>[[%Field:Created%]]</t>
+  </si>
+  <si>
+    <t>TỔNG TIỀN HÀNG</t>
+  </si>
+  <si>
+    <t>[[%Field:PriceVND%]]</t>
+  </si>
+  <si>
+    <t>PHÍ CÂN NẶNG</t>
+  </si>
+  <si>
+    <t>[[%Field:FeeWeight%]]</t>
+  </si>
+  <si>
+    <t>PHỤ PHÍ</t>
+  </si>
+  <si>
+    <t>[[%Field:Surcharge%]]</t>
   </si>
 </sst>
 </file>
@@ -205,9 +217,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -245,7 +257,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -351,7 +363,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,117 +513,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468A229E-F50A-4F33-84FD-61EB5F522203}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="30.88671875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="33.21875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="27.77734375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="30.109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="23.6640625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="22" style="6" customWidth="1"/>
-    <col min="13" max="13" width="25.21875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="25.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="27.88671875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="25.88671875" style="6" customWidth="1"/>
+    <col min="9" max="10" width="30.88671875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="33.21875" style="6" customWidth="1"/>
+    <col min="12" max="12" width="27.77734375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="30.109375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="22" style="6" customWidth="1"/>
+    <col min="16" max="16" width="25.21875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="J1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="J2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="P2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>